<commit_message>
prob id 14~17 완
</commit_message>
<xml_diff>
--- a/확률정보.xlsx
+++ b/확률정보.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\파이썬프로젝트\r2mProbLog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonMsLab\r2mProbLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603F4528-3EB2-4CFD-8446-4754B3914F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C652B780-06F3-4A78-BC9E-7B620BE59534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{ABCE2CA0-A1D3-4D65-96EE-F34166D7733B}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="15435" firstSheet="1" activeTab="1" xr2:uid="{ABCE2CA0-A1D3-4D65-96EE-F34166D7733B}"/>
   </bookViews>
   <sheets>
     <sheet name="23년4월" sheetId="1" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="354">
   <si>
     <t>Category 1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2023,45 +2023,6 @@
     <xf numFmtId="176" fontId="6" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="10" fontId="6" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2079,6 +2040,45 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2531,10 +2531,10 @@
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="107" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -2569,8 +2569,8 @@
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="94"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="103"/>
       <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
@@ -2603,8 +2603,8 @@
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="99"/>
-      <c r="B4" s="94" t="s">
+      <c r="A4" s="100"/>
+      <c r="B4" s="103" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -2639,8 +2639,8 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="99"/>
-      <c r="B5" s="94"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="16" t="s">
         <v>17</v>
       </c>
@@ -2673,8 +2673,8 @@
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="99"/>
-      <c r="B6" s="94" t="s">
+      <c r="A6" s="100"/>
+      <c r="B6" s="103" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -2705,8 +2705,8 @@
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="99"/>
-      <c r="B7" s="94"/>
+      <c r="A7" s="100"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="16" t="s">
         <v>21</v>
       </c>
@@ -2735,8 +2735,8 @@
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="99"/>
-      <c r="B8" s="94"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
@@ -2765,8 +2765,8 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
-      <c r="B9" s="94"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="103"/>
       <c r="C9" s="16" t="s">
         <v>23</v>
       </c>
@@ -2795,8 +2795,8 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="99"/>
-      <c r="B10" s="94"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="16" t="s">
         <v>24</v>
       </c>
@@ -2825,8 +2825,8 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="94"/>
+      <c r="A11" s="100"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="16" t="s">
         <v>25</v>
       </c>
@@ -2859,8 +2859,8 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="99"/>
-      <c r="B12" s="94"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="16" t="s">
         <v>26</v>
       </c>
@@ -2893,8 +2893,8 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="99"/>
-      <c r="B13" s="94"/>
+      <c r="A13" s="100"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="16" t="s">
         <v>27</v>
       </c>
@@ -2927,8 +2927,8 @@
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="99"/>
-      <c r="B14" s="94"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="16" t="s">
         <v>28</v>
       </c>
@@ -2957,8 +2957,8 @@
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="99"/>
-      <c r="B15" s="94"/>
+      <c r="A15" s="100"/>
+      <c r="B15" s="103"/>
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
@@ -2987,8 +2987,8 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="99"/>
-      <c r="B16" s="94"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="16" t="s">
         <v>31</v>
       </c>
@@ -3010,8 +3010,8 @@
       <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="99"/>
-      <c r="B17" s="94" t="s">
+      <c r="A17" s="100"/>
+      <c r="B17" s="103" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -3035,8 +3035,8 @@
       <c r="K17" s="21"/>
     </row>
     <row r="18" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="99"/>
-      <c r="B18" s="94"/>
+      <c r="A18" s="100"/>
+      <c r="B18" s="103"/>
       <c r="C18" s="16" t="s">
         <v>34</v>
       </c>
@@ -3060,8 +3060,8 @@
       <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="99"/>
-      <c r="B19" s="94"/>
+      <c r="A19" s="100"/>
+      <c r="B19" s="103"/>
       <c r="C19" s="16" t="s">
         <v>36</v>
       </c>
@@ -3083,8 +3083,8 @@
       <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="99"/>
-      <c r="B20" s="94"/>
+      <c r="A20" s="100"/>
+      <c r="B20" s="103"/>
       <c r="C20" s="16" t="s">
         <v>38</v>
       </c>
@@ -3106,8 +3106,8 @@
       <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99"/>
-      <c r="B21" s="94"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="103"/>
       <c r="C21" s="16" t="s">
         <v>39</v>
       </c>
@@ -3129,8 +3129,8 @@
       <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="99"/>
-      <c r="B22" s="94"/>
+      <c r="A22" s="100"/>
+      <c r="B22" s="103"/>
       <c r="C22" s="16" t="s">
         <v>40</v>
       </c>
@@ -3152,8 +3152,8 @@
       <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="99"/>
-      <c r="B23" s="94"/>
+      <c r="A23" s="100"/>
+      <c r="B23" s="103"/>
       <c r="C23" s="16" t="s">
         <v>41</v>
       </c>
@@ -3175,8 +3175,8 @@
       <c r="K23" s="21"/>
     </row>
     <row r="24" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="99"/>
-      <c r="B24" s="94"/>
+      <c r="A24" s="100"/>
+      <c r="B24" s="103"/>
       <c r="C24" s="16" t="s">
         <v>42</v>
       </c>
@@ -3198,8 +3198,8 @@
       <c r="K24" s="21"/>
     </row>
     <row r="25" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="99"/>
-      <c r="B25" s="94"/>
+      <c r="A25" s="100"/>
+      <c r="B25" s="103"/>
       <c r="C25" s="16" t="s">
         <v>43</v>
       </c>
@@ -3223,8 +3223,8 @@
       <c r="K25" s="21"/>
     </row>
     <row r="26" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="99"/>
-      <c r="B26" s="94"/>
+      <c r="A26" s="100"/>
+      <c r="B26" s="103"/>
       <c r="C26" s="16" t="s">
         <v>45</v>
       </c>
@@ -3246,8 +3246,8 @@
       <c r="K26" s="21"/>
     </row>
     <row r="27" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="99"/>
-      <c r="B27" s="94"/>
+      <c r="A27" s="100"/>
+      <c r="B27" s="103"/>
       <c r="C27" s="16" t="s">
         <v>46</v>
       </c>
@@ -3269,8 +3269,8 @@
       <c r="K27" s="21"/>
     </row>
     <row r="28" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="99"/>
-      <c r="B28" s="94"/>
+      <c r="A28" s="100"/>
+      <c r="B28" s="103"/>
       <c r="C28" s="16" t="s">
         <v>47</v>
       </c>
@@ -3292,8 +3292,8 @@
       <c r="K28" s="21"/>
     </row>
     <row r="29" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="99"/>
-      <c r="B29" s="94"/>
+      <c r="A29" s="100"/>
+      <c r="B29" s="103"/>
       <c r="C29" s="16" t="s">
         <v>48</v>
       </c>
@@ -3315,8 +3315,8 @@
       <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="99"/>
-      <c r="B30" s="94"/>
+      <c r="A30" s="100"/>
+      <c r="B30" s="103"/>
       <c r="C30" s="16" t="s">
         <v>49</v>
       </c>
@@ -3338,8 +3338,8 @@
       <c r="K30" s="21"/>
     </row>
     <row r="31" spans="1:21" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="99"/>
-      <c r="B31" s="94"/>
+      <c r="A31" s="100"/>
+      <c r="B31" s="103"/>
       <c r="C31" s="16" t="s">
         <v>50</v>
       </c>
@@ -3376,7 +3376,7 @@
       <c r="U31" s="1"/>
     </row>
     <row r="32" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="99"/>
+      <c r="A32" s="100"/>
       <c r="B32" s="15" t="s">
         <v>52</v>
       </c>
@@ -3414,7 +3414,7 @@
       <c r="U32" s="1"/>
     </row>
     <row r="33" spans="1:35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="99"/>
+      <c r="A33" s="100"/>
       <c r="B33" s="15" t="s">
         <v>54</v>
       </c>
@@ -3452,7 +3452,7 @@
       <c r="U33" s="1"/>
     </row>
     <row r="34" spans="1:35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="99"/>
+      <c r="A34" s="100"/>
       <c r="B34" s="15" t="s">
         <v>56</v>
       </c>
@@ -3490,8 +3490,8 @@
       <c r="U34" s="1"/>
     </row>
     <row r="35" spans="1:35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="99"/>
-      <c r="B35" s="94" t="s">
+      <c r="A35" s="100"/>
+      <c r="B35" s="103" t="s">
         <v>58</v>
       </c>
       <c r="C35" s="16" t="s">
@@ -3526,23 +3526,23 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
-      <c r="W35" s="97"/>
-      <c r="X35" s="97"/>
-      <c r="Y35" s="97"/>
-      <c r="Z35" s="97"/>
-      <c r="AA35" s="97"/>
-      <c r="AB35" s="97"/>
-      <c r="AC35" s="97"/>
-      <c r="AD35" s="97"/>
-      <c r="AE35" s="97"/>
-      <c r="AF35" s="97"/>
-      <c r="AG35" s="97"/>
-      <c r="AH35" s="97"/>
-      <c r="AI35" s="97"/>
+      <c r="W35" s="110"/>
+      <c r="X35" s="110"/>
+      <c r="Y35" s="110"/>
+      <c r="Z35" s="110"/>
+      <c r="AA35" s="110"/>
+      <c r="AB35" s="110"/>
+      <c r="AC35" s="110"/>
+      <c r="AD35" s="110"/>
+      <c r="AE35" s="110"/>
+      <c r="AF35" s="110"/>
+      <c r="AG35" s="110"/>
+      <c r="AH35" s="110"/>
+      <c r="AI35" s="110"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A36" s="99"/>
-      <c r="B36" s="94"/>
+      <c r="A36" s="100"/>
+      <c r="B36" s="103"/>
       <c r="C36" s="16" t="s">
         <v>60</v>
       </c>
@@ -3567,23 +3567,23 @@
       </c>
       <c r="K36" s="31"/>
       <c r="V36"/>
-      <c r="W36" s="97"/>
-      <c r="X36" s="97"/>
-      <c r="Y36" s="97"/>
-      <c r="Z36" s="97"/>
-      <c r="AA36" s="97"/>
-      <c r="AB36" s="97"/>
-      <c r="AC36" s="97"/>
-      <c r="AD36" s="97"/>
-      <c r="AE36" s="97"/>
-      <c r="AF36" s="97"/>
-      <c r="AG36" s="97"/>
-      <c r="AH36" s="97"/>
-      <c r="AI36" s="97"/>
+      <c r="W36" s="110"/>
+      <c r="X36" s="110"/>
+      <c r="Y36" s="110"/>
+      <c r="Z36" s="110"/>
+      <c r="AA36" s="110"/>
+      <c r="AB36" s="110"/>
+      <c r="AC36" s="110"/>
+      <c r="AD36" s="110"/>
+      <c r="AE36" s="110"/>
+      <c r="AF36" s="110"/>
+      <c r="AG36" s="110"/>
+      <c r="AH36" s="110"/>
+      <c r="AI36" s="110"/>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A37" s="99"/>
-      <c r="B37" s="94"/>
+      <c r="A37" s="100"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="16" t="s">
         <v>61</v>
       </c>
@@ -3608,22 +3608,22 @@
       </c>
       <c r="K37" s="31"/>
       <c r="V37"/>
-      <c r="W37" s="97"/>
-      <c r="X37" s="97"/>
-      <c r="Y37" s="97"/>
-      <c r="Z37" s="97"/>
-      <c r="AA37" s="97"/>
-      <c r="AB37" s="97"/>
-      <c r="AC37" s="97"/>
-      <c r="AD37" s="97"/>
-      <c r="AE37" s="97"/>
-      <c r="AF37" s="97"/>
-      <c r="AG37" s="97"/>
-      <c r="AH37" s="97"/>
-      <c r="AI37" s="97"/>
+      <c r="W37" s="110"/>
+      <c r="X37" s="110"/>
+      <c r="Y37" s="110"/>
+      <c r="Z37" s="110"/>
+      <c r="AA37" s="110"/>
+      <c r="AB37" s="110"/>
+      <c r="AC37" s="110"/>
+      <c r="AD37" s="110"/>
+      <c r="AE37" s="110"/>
+      <c r="AF37" s="110"/>
+      <c r="AG37" s="110"/>
+      <c r="AH37" s="110"/>
+      <c r="AI37" s="110"/>
     </row>
     <row r="38" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="100"/>
+      <c r="A38" s="102"/>
       <c r="B38" s="32" t="s">
         <v>63</v>
       </c>
@@ -3645,25 +3645,25 @@
       </c>
       <c r="K38" s="39"/>
       <c r="V38"/>
-      <c r="W38" s="97"/>
-      <c r="X38" s="97"/>
-      <c r="Y38" s="97"/>
-      <c r="Z38" s="97"/>
-      <c r="AA38" s="97"/>
-      <c r="AB38" s="97"/>
-      <c r="AC38" s="97"/>
-      <c r="AD38" s="97"/>
-      <c r="AE38" s="97"/>
-      <c r="AF38" s="97"/>
-      <c r="AG38" s="97"/>
-      <c r="AH38" s="97"/>
-      <c r="AI38" s="97"/>
+      <c r="W38" s="110"/>
+      <c r="X38" s="110"/>
+      <c r="Y38" s="110"/>
+      <c r="Z38" s="110"/>
+      <c r="AA38" s="110"/>
+      <c r="AB38" s="110"/>
+      <c r="AC38" s="110"/>
+      <c r="AD38" s="110"/>
+      <c r="AE38" s="110"/>
+      <c r="AF38" s="110"/>
+      <c r="AG38" s="110"/>
+      <c r="AH38" s="110"/>
+      <c r="AI38" s="110"/>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A39" s="98" t="s">
+      <c r="A39" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="93" t="s">
+      <c r="B39" s="107" t="s">
         <v>67</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -3705,8 +3705,8 @@
       <c r="AI39"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A40" s="99"/>
-      <c r="B40" s="94"/>
+      <c r="A40" s="100"/>
+      <c r="B40" s="103"/>
       <c r="C40" s="16" t="s">
         <v>69</v>
       </c>
@@ -3746,8 +3746,8 @@
       <c r="AI40"/>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A41" s="99"/>
-      <c r="B41" s="94" t="s">
+      <c r="A41" s="100"/>
+      <c r="B41" s="103" t="s">
         <v>70</v>
       </c>
       <c r="C41" s="16" t="s">
@@ -3789,8 +3789,8 @@
       <c r="AI41"/>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A42" s="99"/>
-      <c r="B42" s="94"/>
+      <c r="A42" s="100"/>
+      <c r="B42" s="103"/>
       <c r="C42" s="16" t="s">
         <v>72</v>
       </c>
@@ -3832,8 +3832,8 @@
       <c r="AI42"/>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A43" s="99"/>
-      <c r="B43" s="94" t="s">
+      <c r="A43" s="100"/>
+      <c r="B43" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C43" s="16" t="s">
@@ -3862,8 +3862,8 @@
       <c r="Z43"/>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A44" s="99"/>
-      <c r="B44" s="94"/>
+      <c r="A44" s="100"/>
+      <c r="B44" s="103"/>
       <c r="C44" s="16" t="s">
         <v>77</v>
       </c>
@@ -3892,8 +3892,8 @@
       <c r="Z44"/>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A45" s="99"/>
-      <c r="B45" s="94"/>
+      <c r="A45" s="100"/>
+      <c r="B45" s="103"/>
       <c r="C45" s="16" t="s">
         <v>79</v>
       </c>
@@ -3922,8 +3922,8 @@
       <c r="Z45"/>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A46" s="99"/>
-      <c r="B46" s="94"/>
+      <c r="A46" s="100"/>
+      <c r="B46" s="103"/>
       <c r="C46" s="16" t="s">
         <v>80</v>
       </c>
@@ -3952,8 +3952,8 @@
       <c r="Z46"/>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A47" s="99"/>
-      <c r="B47" s="94"/>
+      <c r="A47" s="100"/>
+      <c r="B47" s="103"/>
       <c r="C47" s="16" t="s">
         <v>81</v>
       </c>
@@ -3977,8 +3977,8 @@
       <c r="K47" s="21"/>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A48" s="99"/>
-      <c r="B48" s="94"/>
+      <c r="A48" s="100"/>
+      <c r="B48" s="103"/>
       <c r="C48" s="16" t="s">
         <v>82</v>
       </c>
@@ -4004,8 +4004,8 @@
       <c r="K48" s="21"/>
     </row>
     <row r="49" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A49" s="99"/>
-      <c r="B49" s="94"/>
+      <c r="A49" s="100"/>
+      <c r="B49" s="103"/>
       <c r="C49" s="16" t="s">
         <v>83</v>
       </c>
@@ -4031,8 +4031,8 @@
       <c r="K49" s="21"/>
     </row>
     <row r="50" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A50" s="99"/>
-      <c r="B50" s="94"/>
+      <c r="A50" s="100"/>
+      <c r="B50" s="103"/>
       <c r="C50" s="16" t="s">
         <v>84</v>
       </c>
@@ -4056,8 +4056,8 @@
       <c r="K50" s="21"/>
     </row>
     <row r="51" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A51" s="99"/>
-      <c r="B51" s="94"/>
+      <c r="A51" s="100"/>
+      <c r="B51" s="103"/>
       <c r="C51" s="16" t="s">
         <v>86</v>
       </c>
@@ -4084,8 +4084,8 @@
       <c r="K51" s="21"/>
     </row>
     <row r="52" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A52" s="99"/>
-      <c r="B52" s="94"/>
+      <c r="A52" s="100"/>
+      <c r="B52" s="103"/>
       <c r="C52" s="16" t="s">
         <v>88</v>
       </c>
@@ -4112,8 +4112,8 @@
       <c r="K52" s="21"/>
     </row>
     <row r="53" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="99"/>
-      <c r="B53" s="94"/>
+      <c r="A53" s="100"/>
+      <c r="B53" s="103"/>
       <c r="C53" s="16" t="s">
         <v>89</v>
       </c>
@@ -4170,8 +4170,8 @@
       <c r="AP53" s="1"/>
     </row>
     <row r="54" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="99"/>
-      <c r="B54" s="94" t="s">
+      <c r="A54" s="100"/>
+      <c r="B54" s="103" t="s">
         <v>90</v>
       </c>
       <c r="C54" s="16" t="s">
@@ -4228,8 +4228,8 @@
       <c r="AP54" s="1"/>
     </row>
     <row r="55" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="99"/>
-      <c r="B55" s="94"/>
+      <c r="A55" s="100"/>
+      <c r="B55" s="103"/>
       <c r="C55" s="16" t="s">
         <v>92</v>
       </c>
@@ -4286,8 +4286,8 @@
       <c r="AP55" s="1"/>
     </row>
     <row r="56" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="99"/>
-      <c r="B56" s="94"/>
+      <c r="A56" s="100"/>
+      <c r="B56" s="103"/>
       <c r="C56" s="16" t="s">
         <v>94</v>
       </c>
@@ -4342,8 +4342,8 @@
       <c r="AP56" s="1"/>
     </row>
     <row r="57" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="99"/>
-      <c r="B57" s="94"/>
+      <c r="A57" s="100"/>
+      <c r="B57" s="103"/>
       <c r="C57" s="16" t="s">
         <v>96</v>
       </c>
@@ -4400,8 +4400,8 @@
       <c r="AP57" s="1"/>
     </row>
     <row r="58" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="99"/>
-      <c r="B58" s="94"/>
+      <c r="A58" s="100"/>
+      <c r="B58" s="103"/>
       <c r="C58" s="16" t="s">
         <v>98</v>
       </c>
@@ -4458,8 +4458,8 @@
       <c r="AP58" s="1"/>
     </row>
     <row r="59" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="99"/>
-      <c r="B59" s="94"/>
+      <c r="A59" s="100"/>
+      <c r="B59" s="103"/>
       <c r="C59" s="16" t="s">
         <v>99</v>
       </c>
@@ -4514,8 +4514,8 @@
       <c r="AP59" s="1"/>
     </row>
     <row r="60" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="99"/>
-      <c r="B60" s="94"/>
+      <c r="A60" s="100"/>
+      <c r="B60" s="103"/>
       <c r="C60" s="16" t="s">
         <v>100</v>
       </c>
@@ -4570,8 +4570,8 @@
       <c r="AP60" s="1"/>
     </row>
     <row r="61" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="99"/>
-      <c r="B61" s="94"/>
+      <c r="A61" s="100"/>
+      <c r="B61" s="103"/>
       <c r="C61" s="16" t="s">
         <v>101</v>
       </c>
@@ -4628,8 +4628,8 @@
       <c r="AP61" s="1"/>
     </row>
     <row r="62" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="99"/>
-      <c r="B62" s="94"/>
+      <c r="A62" s="100"/>
+      <c r="B62" s="103"/>
       <c r="C62" s="16" t="s">
         <v>103</v>
       </c>
@@ -4688,8 +4688,8 @@
       <c r="AP62" s="1"/>
     </row>
     <row r="63" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="99"/>
-      <c r="B63" s="94"/>
+      <c r="A63" s="100"/>
+      <c r="B63" s="103"/>
       <c r="C63" s="16" t="s">
         <v>105</v>
       </c>
@@ -4746,8 +4746,8 @@
       <c r="AP63" s="1"/>
     </row>
     <row r="64" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="99"/>
-      <c r="B64" s="94"/>
+      <c r="A64" s="100"/>
+      <c r="B64" s="103"/>
       <c r="C64" s="16" t="s">
         <v>106</v>
       </c>
@@ -4802,8 +4802,8 @@
       <c r="AP64" s="1"/>
     </row>
     <row r="65" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="99"/>
-      <c r="B65" s="94"/>
+      <c r="A65" s="100"/>
+      <c r="B65" s="103"/>
       <c r="C65" s="16" t="s">
         <v>107</v>
       </c>
@@ -4858,8 +4858,8 @@
       <c r="AP65" s="1"/>
     </row>
     <row r="66" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="99"/>
-      <c r="B66" s="94"/>
+      <c r="A66" s="100"/>
+      <c r="B66" s="103"/>
       <c r="C66" s="16" t="s">
         <v>108</v>
       </c>
@@ -4914,8 +4914,8 @@
       <c r="AP66" s="1"/>
     </row>
     <row r="67" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="99"/>
-      <c r="B67" s="94"/>
+      <c r="A67" s="100"/>
+      <c r="B67" s="103"/>
       <c r="C67" s="16" t="s">
         <v>109</v>
       </c>
@@ -4972,8 +4972,8 @@
       <c r="AP67" s="1"/>
     </row>
     <row r="68" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="99"/>
-      <c r="B68" s="94"/>
+      <c r="A68" s="100"/>
+      <c r="B68" s="103"/>
       <c r="C68" s="16" t="s">
         <v>110</v>
       </c>
@@ -5030,7 +5030,7 @@
       <c r="AP68" s="1"/>
     </row>
     <row r="69" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="99"/>
+      <c r="A69" s="100"/>
       <c r="B69" s="15" t="s">
         <v>111</v>
       </c>
@@ -5089,7 +5089,7 @@
       <c r="AP69" s="1"/>
     </row>
     <row r="70" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="99"/>
+      <c r="A70" s="100"/>
       <c r="B70" s="15" t="s">
         <v>113</v>
       </c>
@@ -5148,7 +5148,7 @@
       <c r="AP70" s="1"/>
     </row>
     <row r="71" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="99"/>
+      <c r="A71" s="100"/>
       <c r="B71" s="15" t="s">
         <v>115</v>
       </c>
@@ -5207,7 +5207,7 @@
       <c r="AP71" s="1"/>
     </row>
     <row r="72" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="99"/>
+      <c r="A72" s="100"/>
       <c r="B72" s="15" t="s">
         <v>117</v>
       </c>
@@ -5268,7 +5268,7 @@
       <c r="AP72" s="1"/>
     </row>
     <row r="73" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="99"/>
+      <c r="A73" s="100"/>
       <c r="B73" s="15" t="s">
         <v>119</v>
       </c>
@@ -5327,8 +5327,8 @@
       <c r="AP73" s="1"/>
     </row>
     <row r="74" spans="1:42" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A74" s="99"/>
-      <c r="B74" s="94" t="s">
+      <c r="A74" s="100"/>
+      <c r="B74" s="103" t="s">
         <v>121</v>
       </c>
       <c r="C74" s="16" t="s">
@@ -5388,8 +5388,8 @@
       <c r="AP74" s="1"/>
     </row>
     <row r="75" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="99"/>
-      <c r="B75" s="94"/>
+      <c r="A75" s="100"/>
+      <c r="B75" s="103"/>
       <c r="C75" s="16" t="s">
         <v>125</v>
       </c>
@@ -5447,8 +5447,8 @@
       <c r="AP75" s="1"/>
     </row>
     <row r="76" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="99"/>
-      <c r="B76" s="94"/>
+      <c r="A76" s="100"/>
+      <c r="B76" s="103"/>
       <c r="C76" s="16" t="s">
         <v>127</v>
       </c>
@@ -5504,8 +5504,8 @@
       <c r="AP76" s="1"/>
     </row>
     <row r="77" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="99"/>
-      <c r="B77" s="94"/>
+      <c r="A77" s="100"/>
+      <c r="B77" s="103"/>
       <c r="C77" s="16" t="s">
         <v>128</v>
       </c>
@@ -5561,8 +5561,8 @@
       <c r="AP77" s="1"/>
     </row>
     <row r="78" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="99"/>
-      <c r="B78" s="94"/>
+      <c r="A78" s="100"/>
+      <c r="B78" s="103"/>
       <c r="C78" s="16" t="s">
         <v>129</v>
       </c>
@@ -5618,7 +5618,7 @@
       <c r="AP78" s="1"/>
     </row>
     <row r="79" spans="1:42" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="100"/>
+      <c r="A79" s="102"/>
       <c r="B79" s="32" t="s">
         <v>130</v>
       </c>
@@ -5671,10 +5671,10 @@
       <c r="AP79" s="1"/>
     </row>
     <row r="80" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="98" t="s">
+      <c r="A80" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="93" t="s">
+      <c r="B80" s="107" t="s">
         <v>133</v>
       </c>
       <c r="C80" s="9" t="s">
@@ -5732,8 +5732,8 @@
       <c r="AP80" s="1"/>
     </row>
     <row r="81" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="99"/>
-      <c r="B81" s="94"/>
+      <c r="A81" s="100"/>
+      <c r="B81" s="103"/>
       <c r="C81" s="16" t="s">
         <v>135</v>
       </c>
@@ -5789,8 +5789,8 @@
       <c r="AP81" s="1"/>
     </row>
     <row r="82" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="99"/>
-      <c r="B82" s="94"/>
+      <c r="A82" s="100"/>
+      <c r="B82" s="103"/>
       <c r="C82" s="16" t="s">
         <v>136</v>
       </c>
@@ -5846,8 +5846,8 @@
       <c r="AP82" s="1"/>
     </row>
     <row r="83" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="99"/>
-      <c r="B83" s="94"/>
+      <c r="A83" s="100"/>
+      <c r="B83" s="103"/>
       <c r="C83" s="16" t="s">
         <v>137</v>
       </c>
@@ -5903,8 +5903,8 @@
       <c r="AP83" s="1"/>
     </row>
     <row r="84" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="99"/>
-      <c r="B84" s="94"/>
+      <c r="A84" s="100"/>
+      <c r="B84" s="103"/>
       <c r="C84" s="16" t="s">
         <v>138</v>
       </c>
@@ -5960,8 +5960,8 @@
       <c r="AP84" s="1"/>
     </row>
     <row r="85" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="99"/>
-      <c r="B85" s="94"/>
+      <c r="A85" s="100"/>
+      <c r="B85" s="103"/>
       <c r="C85" s="16" t="s">
         <v>139</v>
       </c>
@@ -6017,8 +6017,8 @@
       <c r="AP85" s="1"/>
     </row>
     <row r="86" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="99"/>
-      <c r="B86" s="94" t="s">
+      <c r="A86" s="100"/>
+      <c r="B86" s="103" t="s">
         <v>140</v>
       </c>
       <c r="C86" s="16" t="s">
@@ -6068,8 +6068,8 @@
       <c r="AP86" s="1"/>
     </row>
     <row r="87" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="99"/>
-      <c r="B87" s="94"/>
+      <c r="A87" s="100"/>
+      <c r="B87" s="103"/>
       <c r="C87" s="16" t="s">
         <v>143</v>
       </c>
@@ -6117,8 +6117,8 @@
       <c r="AP87" s="1"/>
     </row>
     <row r="88" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="99"/>
-      <c r="B88" s="94"/>
+      <c r="A88" s="100"/>
+      <c r="B88" s="103"/>
       <c r="C88" s="16" t="s">
         <v>144</v>
       </c>
@@ -6166,8 +6166,8 @@
       <c r="AP88" s="1"/>
     </row>
     <row r="89" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="99"/>
-      <c r="B89" s="94"/>
+      <c r="A89" s="100"/>
+      <c r="B89" s="103"/>
       <c r="C89" s="16" t="s">
         <v>145</v>
       </c>
@@ -6215,8 +6215,8 @@
       <c r="AP89" s="1"/>
     </row>
     <row r="90" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="99"/>
-      <c r="B90" s="94"/>
+      <c r="A90" s="100"/>
+      <c r="B90" s="103"/>
       <c r="C90" s="16" t="s">
         <v>146</v>
       </c>
@@ -6264,8 +6264,8 @@
       <c r="AP90" s="1"/>
     </row>
     <row r="91" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="99"/>
-      <c r="B91" s="94"/>
+      <c r="A91" s="100"/>
+      <c r="B91" s="103"/>
       <c r="C91" s="16" t="s">
         <v>147</v>
       </c>
@@ -6313,7 +6313,7 @@
       <c r="AP91" s="1"/>
     </row>
     <row r="92" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="99"/>
+      <c r="A92" s="100"/>
       <c r="B92" s="15" t="s">
         <v>148</v>
       </c>
@@ -6364,7 +6364,7 @@
       <c r="AP92" s="1"/>
     </row>
     <row r="93" spans="1:42" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="100"/>
+      <c r="A93" s="102"/>
       <c r="B93" s="32" t="s">
         <v>151</v>
       </c>
@@ -6421,13 +6421,13 @@
       <c r="AP93" s="1"/>
     </row>
     <row r="94" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="98" t="s">
+      <c r="A94" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="B94" s="93" t="s">
+      <c r="B94" s="107" t="s">
         <v>154</v>
       </c>
-      <c r="C94" s="95" t="s">
+      <c r="C94" s="108" t="s">
         <v>155</v>
       </c>
       <c r="D94" s="50"/>
@@ -6476,9 +6476,9 @@
       <c r="AP94" s="1"/>
     </row>
     <row r="95" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="99"/>
-      <c r="B95" s="94"/>
-      <c r="C95" s="96"/>
+      <c r="A95" s="100"/>
+      <c r="B95" s="103"/>
+      <c r="C95" s="109"/>
       <c r="D95" s="24"/>
       <c r="E95" s="18"/>
       <c r="F95" s="18">
@@ -6525,9 +6525,9 @@
       <c r="AP95" s="1"/>
     </row>
     <row r="96" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="99"/>
-      <c r="B96" s="94"/>
-      <c r="C96" s="96"/>
+      <c r="A96" s="100"/>
+      <c r="B96" s="103"/>
+      <c r="C96" s="109"/>
       <c r="D96" s="24"/>
       <c r="E96" s="18"/>
       <c r="F96" s="18">
@@ -6574,9 +6574,9 @@
       <c r="AP96" s="1"/>
     </row>
     <row r="97" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="99"/>
-      <c r="B97" s="94"/>
-      <c r="C97" s="96"/>
+      <c r="A97" s="100"/>
+      <c r="B97" s="103"/>
+      <c r="C97" s="109"/>
       <c r="D97" s="24"/>
       <c r="E97" s="18"/>
       <c r="F97" s="18">
@@ -6623,9 +6623,9 @@
       <c r="AP97" s="1"/>
     </row>
     <row r="98" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="99"/>
-      <c r="B98" s="94"/>
-      <c r="C98" s="96"/>
+      <c r="A98" s="100"/>
+      <c r="B98" s="103"/>
+      <c r="C98" s="109"/>
       <c r="D98" s="24"/>
       <c r="E98" s="18"/>
       <c r="F98" s="18">
@@ -6672,9 +6672,9 @@
       <c r="AP98" s="1"/>
     </row>
     <row r="99" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="99"/>
-      <c r="B99" s="94"/>
-      <c r="C99" s="96"/>
+      <c r="A99" s="100"/>
+      <c r="B99" s="103"/>
+      <c r="C99" s="109"/>
       <c r="D99" s="24"/>
       <c r="E99" s="18"/>
       <c r="F99" s="18">
@@ -6721,9 +6721,9 @@
       <c r="AP99" s="1"/>
     </row>
     <row r="100" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="99"/>
-      <c r="B100" s="94"/>
-      <c r="C100" s="96" t="s">
+      <c r="A100" s="100"/>
+      <c r="B100" s="103"/>
+      <c r="C100" s="109" t="s">
         <v>156</v>
       </c>
       <c r="D100" s="24"/>
@@ -6772,9 +6772,9 @@
       <c r="AP100" s="1"/>
     </row>
     <row r="101" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="99"/>
-      <c r="B101" s="94"/>
-      <c r="C101" s="96"/>
+      <c r="A101" s="100"/>
+      <c r="B101" s="103"/>
+      <c r="C101" s="109"/>
       <c r="D101" s="24"/>
       <c r="E101" s="18"/>
       <c r="F101" s="18">
@@ -6821,9 +6821,9 @@
       <c r="AP101" s="1"/>
     </row>
     <row r="102" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="99"/>
-      <c r="B102" s="94"/>
-      <c r="C102" s="96"/>
+      <c r="A102" s="100"/>
+      <c r="B102" s="103"/>
+      <c r="C102" s="109"/>
       <c r="D102" s="24"/>
       <c r="E102" s="18"/>
       <c r="F102" s="18">
@@ -6870,9 +6870,9 @@
       <c r="AP102" s="1"/>
     </row>
     <row r="103" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="99"/>
-      <c r="B103" s="94"/>
-      <c r="C103" s="96" t="s">
+      <c r="A103" s="100"/>
+      <c r="B103" s="103"/>
+      <c r="C103" s="109" t="s">
         <v>157</v>
       </c>
       <c r="D103" s="24"/>
@@ -6921,9 +6921,9 @@
       <c r="AP103" s="1"/>
     </row>
     <row r="104" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="99"/>
-      <c r="B104" s="94"/>
-      <c r="C104" s="96"/>
+      <c r="A104" s="100"/>
+      <c r="B104" s="103"/>
+      <c r="C104" s="109"/>
       <c r="D104" s="24"/>
       <c r="E104" s="18"/>
       <c r="F104" s="18">
@@ -6970,9 +6970,9 @@
       <c r="AP104" s="1"/>
     </row>
     <row r="105" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="99"/>
-      <c r="B105" s="94"/>
-      <c r="C105" s="96"/>
+      <c r="A105" s="100"/>
+      <c r="B105" s="103"/>
+      <c r="C105" s="109"/>
       <c r="D105" s="24"/>
       <c r="E105" s="18"/>
       <c r="F105" s="18">
@@ -7019,7 +7019,7 @@
       <c r="AP105" s="1"/>
     </row>
     <row r="106" spans="1:42" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="100"/>
+      <c r="A106" s="102"/>
       <c r="B106" s="32" t="s">
         <v>158</v>
       </c>
@@ -7070,10 +7070,10 @@
       <c r="AP106" s="1"/>
     </row>
     <row r="107" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="98" t="s">
+      <c r="A107" s="99" t="s">
         <v>161</v>
       </c>
-      <c r="B107" s="93" t="s">
+      <c r="B107" s="107" t="s">
         <v>162</v>
       </c>
       <c r="C107" s="9" t="s">
@@ -7123,8 +7123,8 @@
       <c r="AP107" s="1"/>
     </row>
     <row r="108" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="99"/>
-      <c r="B108" s="94"/>
+      <c r="A108" s="100"/>
+      <c r="B108" s="103"/>
       <c r="C108" s="16" t="s">
         <v>165</v>
       </c>
@@ -7172,8 +7172,8 @@
       <c r="AP108" s="1"/>
     </row>
     <row r="109" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="99"/>
-      <c r="B109" s="94" t="s">
+      <c r="A109" s="100"/>
+      <c r="B109" s="103" t="s">
         <v>166</v>
       </c>
       <c r="C109" s="16" t="s">
@@ -7223,8 +7223,8 @@
       <c r="AP109" s="1"/>
     </row>
     <row r="110" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="99"/>
-      <c r="B110" s="94"/>
+      <c r="A110" s="100"/>
+      <c r="B110" s="103"/>
       <c r="C110" s="16" t="s">
         <v>168</v>
       </c>
@@ -7272,8 +7272,8 @@
       <c r="AP110" s="1"/>
     </row>
     <row r="111" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="99"/>
-      <c r="B111" s="94" t="s">
+      <c r="A111" s="100"/>
+      <c r="B111" s="103" t="s">
         <v>169</v>
       </c>
       <c r="C111" s="16" t="s">
@@ -7323,8 +7323,8 @@
       <c r="AP111" s="1"/>
     </row>
     <row r="112" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="99"/>
-      <c r="B112" s="94"/>
+      <c r="A112" s="100"/>
+      <c r="B112" s="103"/>
       <c r="C112" s="16" t="s">
         <v>171</v>
       </c>
@@ -7372,8 +7372,8 @@
       <c r="AP112" s="1"/>
     </row>
     <row r="113" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="99"/>
-      <c r="B113" s="94" t="s">
+      <c r="A113" s="100"/>
+      <c r="B113" s="103" t="s">
         <v>172</v>
       </c>
       <c r="C113" s="16" t="s">
@@ -7423,8 +7423,8 @@
       <c r="AP113" s="1"/>
     </row>
     <row r="114" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="99"/>
-      <c r="B114" s="94"/>
+      <c r="A114" s="100"/>
+      <c r="B114" s="103"/>
       <c r="C114" s="16" t="s">
         <v>174</v>
       </c>
@@ -7472,8 +7472,8 @@
       <c r="AP114" s="1"/>
     </row>
     <row r="115" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="99"/>
-      <c r="B115" s="94" t="s">
+      <c r="A115" s="100"/>
+      <c r="B115" s="103" t="s">
         <v>175</v>
       </c>
       <c r="C115" s="16" t="s">
@@ -7523,8 +7523,8 @@
       <c r="AP115" s="1"/>
     </row>
     <row r="116" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="99"/>
-      <c r="B116" s="94"/>
+      <c r="A116" s="100"/>
+      <c r="B116" s="103"/>
       <c r="C116" s="16" t="s">
         <v>177</v>
       </c>
@@ -7572,7 +7572,7 @@
       <c r="AP116" s="1"/>
     </row>
     <row r="117" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="99"/>
+      <c r="A117" s="100"/>
       <c r="B117" s="15" t="s">
         <v>178</v>
       </c>
@@ -7623,7 +7623,7 @@
       <c r="AP117" s="1"/>
     </row>
     <row r="118" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="99"/>
+      <c r="A118" s="100"/>
       <c r="B118" s="51" t="s">
         <v>180</v>
       </c>
@@ -7676,7 +7676,7 @@
       <c r="AP118" s="1"/>
     </row>
     <row r="119" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="99"/>
+      <c r="A119" s="100"/>
       <c r="B119" s="51" t="s">
         <v>183</v>
       </c>
@@ -7729,7 +7729,7 @@
       <c r="AP119" s="1"/>
     </row>
     <row r="120" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="99"/>
+      <c r="A120" s="100"/>
       <c r="B120" s="51" t="s">
         <v>185</v>
       </c>
@@ -7782,7 +7782,7 @@
       <c r="AP120" s="1"/>
     </row>
     <row r="121" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="99"/>
+      <c r="A121" s="100"/>
       <c r="B121" s="51" t="s">
         <v>187</v>
       </c>
@@ -7835,7 +7835,7 @@
       <c r="AP121" s="1"/>
     </row>
     <row r="122" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="99"/>
+      <c r="A122" s="100"/>
       <c r="B122" s="51" t="s">
         <v>189</v>
       </c>
@@ -7888,7 +7888,7 @@
       <c r="AP122" s="1"/>
     </row>
     <row r="123" spans="1:42" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="100"/>
+      <c r="A123" s="102"/>
       <c r="B123" s="53" t="s">
         <v>191</v>
       </c>
@@ -7941,7 +7941,7 @@
       <c r="AP123" s="1"/>
     </row>
     <row r="124" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="98" t="s">
+      <c r="A124" s="99" t="s">
         <v>193</v>
       </c>
       <c r="B124" s="8" t="s">
@@ -7994,7 +7994,7 @@
       <c r="AP124" s="1"/>
     </row>
     <row r="125" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="99"/>
+      <c r="A125" s="100"/>
       <c r="B125" s="15" t="s">
         <v>196</v>
       </c>
@@ -8049,7 +8049,7 @@
       <c r="AP125" s="1"/>
     </row>
     <row r="126" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="99"/>
+      <c r="A126" s="100"/>
       <c r="B126" s="15" t="s">
         <v>201</v>
       </c>
@@ -8102,8 +8102,8 @@
       <c r="AP126" s="1"/>
     </row>
     <row r="127" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="99"/>
-      <c r="B127" s="94" t="s">
+      <c r="A127" s="100"/>
+      <c r="B127" s="103" t="s">
         <v>205</v>
       </c>
       <c r="C127" s="16" t="s">
@@ -8153,8 +8153,8 @@
       <c r="AP127" s="1"/>
     </row>
     <row r="128" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="99"/>
-      <c r="B128" s="94"/>
+      <c r="A128" s="100"/>
+      <c r="B128" s="103"/>
       <c r="C128" s="16" t="s">
         <v>208</v>
       </c>
@@ -8202,8 +8202,8 @@
       <c r="AP128" s="1"/>
     </row>
     <row r="129" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="99"/>
-      <c r="B129" s="94"/>
+      <c r="A129" s="100"/>
+      <c r="B129" s="103"/>
       <c r="C129" s="16" t="s">
         <v>210</v>
       </c>
@@ -8251,8 +8251,8 @@
       <c r="AP129" s="1"/>
     </row>
     <row r="130" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="99"/>
-      <c r="B130" s="102" t="s">
+      <c r="A130" s="100"/>
+      <c r="B130" s="104" t="s">
         <v>211</v>
       </c>
       <c r="C130" s="52" t="s">
@@ -8306,8 +8306,8 @@
       <c r="AP130" s="1"/>
     </row>
     <row r="131" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="99"/>
-      <c r="B131" s="102"/>
+      <c r="A131" s="100"/>
+      <c r="B131" s="104"/>
       <c r="C131" s="52" t="s">
         <v>216</v>
       </c>
@@ -8359,8 +8359,8 @@
       <c r="AP131" s="1"/>
     </row>
     <row r="132" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="99"/>
-      <c r="B132" s="94" t="s">
+      <c r="A132" s="100"/>
+      <c r="B132" s="103" t="s">
         <v>217</v>
       </c>
       <c r="C132" s="16" t="s">
@@ -8416,8 +8416,8 @@
       <c r="AP132" s="1"/>
     </row>
     <row r="133" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="99"/>
-      <c r="B133" s="94"/>
+      <c r="A133" s="100"/>
+      <c r="B133" s="103"/>
       <c r="C133" s="16" t="s">
         <v>219</v>
       </c>
@@ -8471,8 +8471,8 @@
       <c r="AP133" s="1"/>
     </row>
     <row r="134" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="99"/>
-      <c r="B134" s="94"/>
+      <c r="A134" s="100"/>
+      <c r="B134" s="103"/>
       <c r="C134" s="16" t="s">
         <v>220</v>
       </c>
@@ -8526,8 +8526,8 @@
       <c r="AP134" s="1"/>
     </row>
     <row r="135" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="99"/>
-      <c r="B135" s="94"/>
+      <c r="A135" s="100"/>
+      <c r="B135" s="103"/>
       <c r="C135" s="16" t="s">
         <v>221</v>
       </c>
@@ -8581,8 +8581,8 @@
       <c r="AP135" s="1"/>
     </row>
     <row r="136" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="99"/>
-      <c r="B136" s="94"/>
+      <c r="A136" s="100"/>
+      <c r="B136" s="103"/>
       <c r="C136" s="16" t="s">
         <v>222</v>
       </c>
@@ -8636,8 +8636,8 @@
       <c r="AP136" s="1"/>
     </row>
     <row r="137" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="99"/>
-      <c r="B137" s="94"/>
+      <c r="A137" s="100"/>
+      <c r="B137" s="103"/>
       <c r="C137" s="16" t="s">
         <v>223</v>
       </c>
@@ -8692,7 +8692,7 @@
     </row>
     <row r="138" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="101"/>
-      <c r="B138" s="103"/>
+      <c r="B138" s="105"/>
       <c r="C138" s="55" t="s">
         <v>224</v>
       </c>
@@ -8747,7 +8747,7 @@
     </row>
     <row r="139" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="101"/>
-      <c r="B139" s="103"/>
+      <c r="B139" s="105"/>
       <c r="C139" s="55" t="s">
         <v>227</v>
       </c>
@@ -8802,7 +8802,7 @@
     </row>
     <row r="140" spans="1:42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="101"/>
-      <c r="B140" s="103"/>
+      <c r="B140" s="105"/>
       <c r="C140" s="55" t="s">
         <v>229</v>
       </c>
@@ -8856,8 +8856,8 @@
       <c r="AP140" s="1"/>
     </row>
     <row r="141" spans="1:42" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="100"/>
-      <c r="B141" s="104"/>
+      <c r="A141" s="102"/>
+      <c r="B141" s="106"/>
       <c r="C141" s="33" t="s">
         <v>230</v>
       </c>
@@ -8913,16 +8913,11 @@
   </sheetData>
   <autoFilter ref="A1:K141" xr:uid="{9C6DE4F0-FB08-4A38-9A04-A033331CA2DF}"/>
   <mergeCells count="31">
-    <mergeCell ref="A124:A141"/>
-    <mergeCell ref="B127:B129"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="B132:B141"/>
-    <mergeCell ref="A107:A123"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="B17:B31"/>
+    <mergeCell ref="B35:B37"/>
     <mergeCell ref="C94:C99"/>
     <mergeCell ref="C100:C102"/>
     <mergeCell ref="C103:C105"/>
@@ -8939,11 +8934,16 @@
     <mergeCell ref="A94:A106"/>
     <mergeCell ref="B94:B105"/>
     <mergeCell ref="A2:A38"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B31"/>
-    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A124:A141"/>
+    <mergeCell ref="B127:B129"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="B132:B141"/>
+    <mergeCell ref="A107:A123"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="B115:B116"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H2:I141">
@@ -8961,14 +8961,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58870481-4012-4967-9DF8-188DDC2BA7B8}">
-  <sheetPr codeName="Sheet2" filterMode="1">
+  <sheetPr codeName="Sheet2">
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:AS143"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H136" sqref="H136"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11:F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9054,7 +9054,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="67" t="s">
         <v>271</v>
@@ -9107,7 +9107,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="67" t="s">
         <v>272</v>
@@ -9157,7 +9157,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="67" t="s">
         <v>16</v>
@@ -9208,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="67" t="s">
         <v>273</v>
@@ -9258,7 +9258,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="67" t="s">
         <v>274</v>
@@ -9305,7 +9305,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="67" t="s">
         <v>275</v>
@@ -9352,7 +9352,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="67" t="s">
         <v>276</v>
@@ -9399,7 +9399,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="67" t="s">
         <v>277</v>
@@ -9446,7 +9446,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="67" t="s">
         <v>278</v>
@@ -9493,7 +9493,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="67" t="s">
         <v>25</v>
@@ -9544,7 +9544,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="67" t="s">
         <v>26</v>
@@ -9595,7 +9595,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="67" t="s">
         <v>27</v>
@@ -9631,7 +9631,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:21" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="65" t="s">
         <v>341</v>
       </c>
@@ -9678,7 +9678,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="65" t="s">
         <v>341</v>
       </c>
@@ -9725,7 +9725,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="65" t="s">
         <v>341</v>
       </c>
@@ -9765,7 +9765,7 @@
       </c>
       <c r="N16" s="73"/>
     </row>
-    <row r="17" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="65" t="s">
         <v>341</v>
       </c>
@@ -9804,7 +9804,7 @@
       </c>
       <c r="N17" s="73"/>
     </row>
-    <row r="18" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="65" t="s">
         <v>341</v>
       </c>
@@ -9846,7 +9846,7 @@
       </c>
       <c r="N18" s="73"/>
     </row>
-    <row r="19" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="65" t="s">
         <v>341</v>
       </c>
@@ -9886,7 +9886,7 @@
       </c>
       <c r="N19" s="73"/>
     </row>
-    <row r="20" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="65" t="s">
         <v>341</v>
       </c>
@@ -9926,7 +9926,7 @@
       </c>
       <c r="N20" s="73"/>
     </row>
-    <row r="21" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="65" t="s">
         <v>341</v>
       </c>
@@ -9966,7 +9966,7 @@
       </c>
       <c r="N21" s="73"/>
     </row>
-    <row r="22" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="65" t="s">
         <v>341</v>
       </c>
@@ -10006,7 +10006,7 @@
       </c>
       <c r="N22" s="73"/>
     </row>
-    <row r="23" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="65" t="s">
         <v>341</v>
       </c>
@@ -10046,7 +10046,7 @@
       </c>
       <c r="N23" s="73"/>
     </row>
-    <row r="24" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="65" t="s">
         <v>341</v>
       </c>
@@ -10086,7 +10086,7 @@
       </c>
       <c r="N24" s="73"/>
     </row>
-    <row r="25" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="65" t="s">
         <v>341</v>
       </c>
@@ -10128,7 +10128,7 @@
       </c>
       <c r="N25" s="73"/>
     </row>
-    <row r="26" spans="1:24" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="65" t="s">
         <v>341</v>
       </c>
@@ -10168,7 +10168,7 @@
       </c>
       <c r="N26" s="73"/>
     </row>
-    <row r="27" spans="1:24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="65" t="s">
         <v>341</v>
       </c>
@@ -10208,7 +10208,7 @@
       </c>
       <c r="N27" s="73"/>
     </row>
-    <row r="28" spans="1:24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="65" t="s">
         <v>341</v>
       </c>
@@ -10248,7 +10248,7 @@
       </c>
       <c r="N28" s="73"/>
     </row>
-    <row r="29" spans="1:24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="65" t="s">
         <v>341</v>
       </c>
@@ -10288,7 +10288,7 @@
       </c>
       <c r="N29" s="73"/>
     </row>
-    <row r="30" spans="1:24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="65" t="s">
         <v>341</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>14</v>
       </c>
       <c r="E31" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="67" t="s">
         <v>310</v>
@@ -10397,7 +10397,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" s="67" t="s">
         <v>279</v>
@@ -10449,7 +10449,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="67" t="s">
         <v>311</v>
@@ -10501,7 +10501,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="67" t="s">
         <v>312</v>
@@ -10553,7 +10553,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="67" t="s">
         <v>313</v>
@@ -10590,19 +10590,19 @@
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
-      <c r="Z35" s="97"/>
-      <c r="AA35" s="97"/>
-      <c r="AB35" s="97"/>
-      <c r="AC35" s="97"/>
-      <c r="AD35" s="97"/>
-      <c r="AE35" s="97"/>
-      <c r="AF35" s="97"/>
-      <c r="AG35" s="97"/>
-      <c r="AH35" s="97"/>
-      <c r="AI35" s="97"/>
-      <c r="AJ35" s="97"/>
-      <c r="AK35" s="97"/>
-      <c r="AL35" s="97"/>
+      <c r="Z35" s="110"/>
+      <c r="AA35" s="110"/>
+      <c r="AB35" s="110"/>
+      <c r="AC35" s="110"/>
+      <c r="AD35" s="110"/>
+      <c r="AE35" s="110"/>
+      <c r="AF35" s="110"/>
+      <c r="AG35" s="110"/>
+      <c r="AH35" s="110"/>
+      <c r="AI35" s="110"/>
+      <c r="AJ35" s="110"/>
+      <c r="AK35" s="110"/>
+      <c r="AL35" s="110"/>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A36" s="65" t="s">
@@ -10619,7 +10619,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" s="67" t="s">
         <v>314</v>
@@ -10648,19 +10648,19 @@
       </c>
       <c r="N36" s="79"/>
       <c r="Y36"/>
-      <c r="Z36" s="97"/>
-      <c r="AA36" s="97"/>
-      <c r="AB36" s="97"/>
-      <c r="AC36" s="97"/>
-      <c r="AD36" s="97"/>
-      <c r="AE36" s="97"/>
-      <c r="AF36" s="97"/>
-      <c r="AG36" s="97"/>
-      <c r="AH36" s="97"/>
-      <c r="AI36" s="97"/>
-      <c r="AJ36" s="97"/>
-      <c r="AK36" s="97"/>
-      <c r="AL36" s="97"/>
+      <c r="Z36" s="110"/>
+      <c r="AA36" s="110"/>
+      <c r="AB36" s="110"/>
+      <c r="AC36" s="110"/>
+      <c r="AD36" s="110"/>
+      <c r="AE36" s="110"/>
+      <c r="AF36" s="110"/>
+      <c r="AG36" s="110"/>
+      <c r="AH36" s="110"/>
+      <c r="AI36" s="110"/>
+      <c r="AJ36" s="110"/>
+      <c r="AK36" s="110"/>
+      <c r="AL36" s="110"/>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A37" s="65" t="s">
@@ -10677,7 +10677,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="67" t="s">
         <v>315</v>
@@ -10706,19 +10706,19 @@
       </c>
       <c r="N37" s="79"/>
       <c r="Y37"/>
-      <c r="Z37" s="97"/>
-      <c r="AA37" s="97"/>
-      <c r="AB37" s="97"/>
-      <c r="AC37" s="97"/>
-      <c r="AD37" s="97"/>
-      <c r="AE37" s="97"/>
-      <c r="AF37" s="97"/>
-      <c r="AG37" s="97"/>
-      <c r="AH37" s="97"/>
-      <c r="AI37" s="97"/>
-      <c r="AJ37" s="97"/>
-      <c r="AK37" s="97"/>
-      <c r="AL37" s="97"/>
+      <c r="Z37" s="110"/>
+      <c r="AA37" s="110"/>
+      <c r="AB37" s="110"/>
+      <c r="AC37" s="110"/>
+      <c r="AD37" s="110"/>
+      <c r="AE37" s="110"/>
+      <c r="AF37" s="110"/>
+      <c r="AG37" s="110"/>
+      <c r="AH37" s="110"/>
+      <c r="AI37" s="110"/>
+      <c r="AJ37" s="110"/>
+      <c r="AK37" s="110"/>
+      <c r="AL37" s="110"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A38" s="65" t="s">
@@ -10735,7 +10735,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" s="67" t="s">
         <v>316</v>
@@ -10762,21 +10762,21 @@
       </c>
       <c r="N38" s="73"/>
       <c r="Y38"/>
-      <c r="Z38" s="97"/>
-      <c r="AA38" s="97"/>
-      <c r="AB38" s="97"/>
-      <c r="AC38" s="97"/>
-      <c r="AD38" s="97"/>
-      <c r="AE38" s="97"/>
-      <c r="AF38" s="97"/>
-      <c r="AG38" s="97"/>
-      <c r="AH38" s="97"/>
-      <c r="AI38" s="97"/>
-      <c r="AJ38" s="97"/>
-      <c r="AK38" s="97"/>
-      <c r="AL38" s="97"/>
-    </row>
-    <row r="39" spans="1:38" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Z38" s="110"/>
+      <c r="AA38" s="110"/>
+      <c r="AB38" s="110"/>
+      <c r="AC38" s="110"/>
+      <c r="AD38" s="110"/>
+      <c r="AE38" s="110"/>
+      <c r="AF38" s="110"/>
+      <c r="AG38" s="110"/>
+      <c r="AH38" s="110"/>
+      <c r="AI38" s="110"/>
+      <c r="AJ38" s="110"/>
+      <c r="AK38" s="110"/>
+      <c r="AL38" s="110"/>
+    </row>
+    <row r="39" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="65" t="s">
         <v>341</v>
       </c>
@@ -10814,19 +10814,19 @@
       </c>
       <c r="N39" s="73"/>
       <c r="Y39"/>
-      <c r="Z39" s="97"/>
-      <c r="AA39" s="97"/>
-      <c r="AB39" s="97"/>
-      <c r="AC39" s="97"/>
-      <c r="AD39" s="97"/>
-      <c r="AE39" s="97"/>
-      <c r="AF39" s="97"/>
-      <c r="AG39" s="97"/>
-      <c r="AH39" s="97"/>
-      <c r="AI39" s="97"/>
-      <c r="AJ39" s="97"/>
-      <c r="AK39" s="97"/>
-      <c r="AL39" s="97"/>
+      <c r="Z39" s="110"/>
+      <c r="AA39" s="110"/>
+      <c r="AB39" s="110"/>
+      <c r="AC39" s="110"/>
+      <c r="AD39" s="110"/>
+      <c r="AE39" s="110"/>
+      <c r="AF39" s="110"/>
+      <c r="AG39" s="110"/>
+      <c r="AH39" s="110"/>
+      <c r="AI39" s="110"/>
+      <c r="AJ39" s="110"/>
+      <c r="AK39" s="110"/>
+      <c r="AL39" s="110"/>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A40" s="81" t="s">
@@ -10842,7 +10842,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="67" t="s">
         <v>280</v>
@@ -10898,7 +10898,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="67" t="s">
         <v>281</v>
@@ -10953,7 +10953,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="67" t="s">
         <v>71</v>
@@ -11009,7 +11009,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="67" t="s">
         <v>282</v>
@@ -11066,7 +11066,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="67" t="s">
         <v>283</v>
@@ -11109,7 +11109,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="67" t="s">
         <v>284</v>
@@ -11154,7 +11154,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="67" t="s">
         <v>285</v>
@@ -11199,7 +11199,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="67" t="s">
         <v>286</v>
@@ -11244,7 +11244,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" s="67" t="s">
         <v>287</v>
@@ -11284,7 +11284,7 @@
         <v>5</v>
       </c>
       <c r="E49" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="67" t="s">
         <v>82</v>
@@ -11326,7 +11326,7 @@
         <v>6</v>
       </c>
       <c r="E50" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" s="67" t="s">
         <v>83</v>
@@ -11368,7 +11368,7 @@
         <v>7</v>
       </c>
       <c r="E51" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" s="67" t="s">
         <v>84</v>
@@ -11395,7 +11395,7 @@
       </c>
       <c r="N51" s="73"/>
     </row>
-    <row r="52" spans="1:45" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="81" t="s">
         <v>66</v>
       </c>
@@ -11439,7 +11439,7 @@
       </c>
       <c r="N52" s="73"/>
     </row>
-    <row r="53" spans="1:45" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="81" t="s">
         <v>66</v>
       </c>
@@ -11483,7 +11483,7 @@
       </c>
       <c r="N53" s="73"/>
     </row>
-    <row r="54" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="81" t="s">
         <v>66</v>
       </c>
@@ -11557,7 +11557,7 @@
       <c r="AR54" s="1"/>
       <c r="AS54" s="1"/>
     </row>
-    <row r="55" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="81" t="s">
         <v>66</v>
       </c>
@@ -11628,7 +11628,7 @@
       <c r="AR55" s="1"/>
       <c r="AS55" s="1"/>
     </row>
-    <row r="56" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="81" t="s">
         <v>66</v>
       </c>
@@ -11702,7 +11702,7 @@
       <c r="AR56" s="1"/>
       <c r="AS56" s="1"/>
     </row>
-    <row r="57" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="81" t="s">
         <v>66</v>
       </c>
@@ -11774,7 +11774,7 @@
       <c r="AR57" s="1"/>
       <c r="AS57" s="1"/>
     </row>
-    <row r="58" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="81" t="s">
         <v>66</v>
       </c>
@@ -11848,7 +11848,7 @@
       <c r="AR58" s="1"/>
       <c r="AS58" s="1"/>
     </row>
-    <row r="59" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="81" t="s">
         <v>66</v>
       </c>
@@ -11922,7 +11922,7 @@
       <c r="AR59" s="1"/>
       <c r="AS59" s="1"/>
     </row>
-    <row r="60" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="81" t="s">
         <v>66</v>
       </c>
@@ -11994,7 +11994,7 @@
       <c r="AR60" s="1"/>
       <c r="AS60" s="1"/>
     </row>
-    <row r="61" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="81" t="s">
         <v>66</v>
       </c>
@@ -12066,7 +12066,7 @@
       <c r="AR61" s="1"/>
       <c r="AS61" s="1"/>
     </row>
-    <row r="62" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="81" t="s">
         <v>66</v>
       </c>
@@ -12140,7 +12140,7 @@
       <c r="AR62" s="1"/>
       <c r="AS62" s="1"/>
     </row>
-    <row r="63" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="81" t="s">
         <v>66</v>
       </c>
@@ -12214,7 +12214,7 @@
       <c r="AR63" s="1"/>
       <c r="AS63" s="1"/>
     </row>
-    <row r="64" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="81" t="s">
         <v>66</v>
       </c>
@@ -12288,7 +12288,7 @@
       <c r="AR64" s="1"/>
       <c r="AS64" s="1"/>
     </row>
-    <row r="65" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="81" t="s">
         <v>66</v>
       </c>
@@ -12360,7 +12360,7 @@
       <c r="AR65" s="1"/>
       <c r="AS65" s="1"/>
     </row>
-    <row r="66" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="81" t="s">
         <v>66</v>
       </c>
@@ -12432,7 +12432,7 @@
       <c r="AR66" s="1"/>
       <c r="AS66" s="1"/>
     </row>
-    <row r="67" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="81" t="s">
         <v>66</v>
       </c>
@@ -12504,7 +12504,7 @@
       <c r="AR67" s="1"/>
       <c r="AS67" s="1"/>
     </row>
-    <row r="68" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="81" t="s">
         <v>66</v>
       </c>
@@ -12578,7 +12578,7 @@
       <c r="AR68" s="1"/>
       <c r="AS68" s="1"/>
     </row>
-    <row r="69" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="81" t="s">
         <v>66</v>
       </c>
@@ -12666,7 +12666,7 @@
         <v>0</v>
       </c>
       <c r="E70" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" s="67" t="s">
         <v>288</v>
@@ -12737,7 +12737,7 @@
         <v>0</v>
       </c>
       <c r="E71" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" s="67" t="s">
         <v>289</v>
@@ -12808,7 +12808,7 @@
         <v>0</v>
       </c>
       <c r="E72" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" s="67" t="s">
         <v>290</v>
@@ -12879,7 +12879,7 @@
         <v>0</v>
       </c>
       <c r="E73" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" s="67" t="s">
         <v>325</v>
@@ -12952,7 +12952,7 @@
         <v>0</v>
       </c>
       <c r="E74" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" s="67" t="s">
         <v>120</v>
@@ -13013,32 +13013,34 @@
       <c r="A75" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="B75" s="106" t="s">
+      <c r="B75" s="93" t="s">
         <v>121</v>
       </c>
-      <c r="C75" s="107"/>
-      <c r="D75" s="107"/>
-      <c r="E75" s="107"/>
-      <c r="F75" s="108" t="s">
+      <c r="C75" s="94"/>
+      <c r="D75" s="94"/>
+      <c r="E75" s="92">
+        <v>0</v>
+      </c>
+      <c r="F75" s="95" t="s">
         <v>326</v>
       </c>
       <c r="G75" s="68">
         <v>44887</v>
       </c>
-      <c r="H75" s="109"/>
-      <c r="I75" s="109"/>
+      <c r="H75" s="96"/>
+      <c r="I75" s="96"/>
       <c r="J75" s="70"/>
-      <c r="K75" s="110" t="s">
+      <c r="K75" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="L75" s="110">
+      <c r="L75" s="97">
         <f>_xlfn.XLOOKUP(K75,타입분류!$A$1:$A$28,타입분류!$B$1:$B$28)</f>
         <v>1</v>
       </c>
-      <c r="M75" s="110" t="s">
+      <c r="M75" s="97" t="s">
         <v>268</v>
       </c>
-      <c r="N75" s="111" t="s">
+      <c r="N75" s="98" t="s">
         <v>353</v>
       </c>
       <c r="P75" s="1"/>
@@ -13086,7 +13088,7 @@
         <v>0</v>
       </c>
       <c r="E76" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" s="67" t="s">
         <v>327</v>
@@ -13159,7 +13161,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="67" t="s">
         <v>328</v>
@@ -13230,7 +13232,7 @@
         <v>2</v>
       </c>
       <c r="E78" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" s="67" t="s">
         <v>329</v>
@@ -13301,7 +13303,7 @@
         <v>3</v>
       </c>
       <c r="E79" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79" s="67" t="s">
         <v>330</v>
@@ -13358,7 +13360,7 @@
       <c r="AR79" s="1"/>
       <c r="AS79" s="1"/>
     </row>
-    <row r="80" spans="1:45" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:45" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="81" t="s">
         <v>66</v>
       </c>
@@ -13441,7 +13443,7 @@
         <v>0</v>
       </c>
       <c r="E81" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" s="67" t="s">
         <v>134</v>
@@ -13513,7 +13515,7 @@
         <v>1</v>
       </c>
       <c r="E82" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82" s="67" t="s">
         <v>135</v>
@@ -13585,7 +13587,7 @@
         <v>2</v>
       </c>
       <c r="E83" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" s="67" t="s">
         <v>136</v>
@@ -13657,7 +13659,7 @@
         <v>3</v>
       </c>
       <c r="E84" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F84" s="67" t="s">
         <v>137</v>
@@ -13729,7 +13731,7 @@
         <v>4</v>
       </c>
       <c r="E85" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" s="67" t="s">
         <v>138</v>
@@ -13801,7 +13803,7 @@
         <v>5</v>
       </c>
       <c r="E86" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F86" s="67" t="s">
         <v>139</v>
@@ -13858,7 +13860,7 @@
       <c r="AR86" s="1"/>
       <c r="AS86" s="1"/>
     </row>
-    <row r="87" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="65" t="s">
         <v>342</v>
       </c>
@@ -13925,7 +13927,7 @@
       <c r="AR87" s="1"/>
       <c r="AS87" s="1"/>
     </row>
-    <row r="88" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="65" t="s">
         <v>342</v>
       </c>
@@ -13993,7 +13995,7 @@
       <c r="AR88" s="1"/>
       <c r="AS88" s="1"/>
     </row>
-    <row r="89" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="65" t="s">
         <v>342</v>
       </c>
@@ -14061,7 +14063,7 @@
       <c r="AR89" s="1"/>
       <c r="AS89" s="1"/>
     </row>
-    <row r="90" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="65" t="s">
         <v>342</v>
       </c>
@@ -14129,7 +14131,7 @@
       <c r="AR90" s="1"/>
       <c r="AS90" s="1"/>
     </row>
-    <row r="91" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="65" t="s">
         <v>342</v>
       </c>
@@ -14197,7 +14199,7 @@
       <c r="AR91" s="1"/>
       <c r="AS91" s="1"/>
     </row>
-    <row r="92" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="65" t="s">
         <v>342</v>
       </c>
@@ -14265,7 +14267,7 @@
       <c r="AR92" s="1"/>
       <c r="AS92" s="1"/>
     </row>
-    <row r="93" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="65" t="s">
         <v>342</v>
       </c>
@@ -14346,7 +14348,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" s="67" t="s">
         <v>152</v>
@@ -14415,9 +14417,9 @@
         <v>0</v>
       </c>
       <c r="E95" s="92">
-        <v>1</v>
-      </c>
-      <c r="F95" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="F95" s="111" t="s">
         <v>155</v>
       </c>
       <c r="G95" s="75"/>
@@ -14483,9 +14485,9 @@
         <v>0</v>
       </c>
       <c r="E96" s="92">
-        <v>1</v>
-      </c>
-      <c r="F96" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F96" s="111"/>
       <c r="G96" s="75"/>
       <c r="H96" s="69">
         <v>1110035</v>
@@ -14549,9 +14551,9 @@
         <v>0</v>
       </c>
       <c r="E97" s="92">
-        <v>1</v>
-      </c>
-      <c r="F97" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F97" s="111"/>
       <c r="G97" s="75"/>
       <c r="H97" s="69">
         <v>1110062</v>
@@ -14615,9 +14617,9 @@
         <v>0</v>
       </c>
       <c r="E98" s="92">
-        <v>1</v>
-      </c>
-      <c r="F98" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F98" s="111"/>
       <c r="G98" s="75"/>
       <c r="H98" s="69">
         <v>502634</v>
@@ -14681,9 +14683,9 @@
         <v>0</v>
       </c>
       <c r="E99" s="92">
-        <v>1</v>
-      </c>
-      <c r="F99" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="111"/>
       <c r="G99" s="75"/>
       <c r="H99" s="69">
         <v>1110036</v>
@@ -14747,9 +14749,9 @@
         <v>0</v>
       </c>
       <c r="E100" s="92">
-        <v>1</v>
-      </c>
-      <c r="F100" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F100" s="111"/>
       <c r="G100" s="75"/>
       <c r="H100" s="69">
         <v>1110061</v>
@@ -14813,9 +14815,9 @@
         <v>1</v>
       </c>
       <c r="E101" s="92">
-        <v>1</v>
-      </c>
-      <c r="F101" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="F101" s="111" t="s">
         <v>156</v>
       </c>
       <c r="G101" s="75"/>
@@ -14881,9 +14883,9 @@
         <v>1</v>
       </c>
       <c r="E102" s="92">
-        <v>1</v>
-      </c>
-      <c r="F102" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F102" s="111"/>
       <c r="G102" s="75"/>
       <c r="H102" s="69">
         <v>502655</v>
@@ -14947,9 +14949,9 @@
         <v>1</v>
       </c>
       <c r="E103" s="92">
-        <v>1</v>
-      </c>
-      <c r="F103" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F103" s="111"/>
       <c r="G103" s="75"/>
       <c r="H103" s="69">
         <v>502657</v>
@@ -15013,9 +15015,9 @@
         <v>2</v>
       </c>
       <c r="E104" s="92">
-        <v>1</v>
-      </c>
-      <c r="F104" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="F104" s="111" t="s">
         <v>157</v>
       </c>
       <c r="G104" s="75"/>
@@ -15081,9 +15083,9 @@
         <v>2</v>
       </c>
       <c r="E105" s="92">
-        <v>1</v>
-      </c>
-      <c r="F105" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F105" s="111"/>
       <c r="G105" s="75"/>
       <c r="H105" s="69">
         <v>502656</v>
@@ -15147,9 +15149,9 @@
         <v>2</v>
       </c>
       <c r="E106" s="92">
-        <v>1</v>
-      </c>
-      <c r="F106" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="F106" s="111"/>
       <c r="G106" s="75"/>
       <c r="H106" s="69">
         <v>502658</v>
@@ -15198,7 +15200,7 @@
       <c r="AR106" s="1"/>
       <c r="AS106" s="1"/>
     </row>
-    <row r="107" spans="1:45" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:45" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="81" t="s">
         <v>343</v>
       </c>
@@ -15265,7 +15267,7 @@
       <c r="AR107" s="1"/>
       <c r="AS107" s="1"/>
     </row>
-    <row r="108" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="65" t="s">
         <v>161</v>
       </c>
@@ -15332,7 +15334,7 @@
       <c r="AR108" s="1"/>
       <c r="AS108" s="1"/>
     </row>
-    <row r="109" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="65" t="s">
         <v>344</v>
       </c>
@@ -15400,7 +15402,7 @@
       <c r="AR109" s="1"/>
       <c r="AS109" s="1"/>
     </row>
-    <row r="110" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="65" t="s">
         <v>344</v>
       </c>
@@ -15467,7 +15469,7 @@
       <c r="AR110" s="1"/>
       <c r="AS110" s="1"/>
     </row>
-    <row r="111" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="65" t="s">
         <v>344</v>
       </c>
@@ -15535,7 +15537,7 @@
       <c r="AR111" s="1"/>
       <c r="AS111" s="1"/>
     </row>
-    <row r="112" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="65" t="s">
         <v>344</v>
       </c>
@@ -15602,7 +15604,7 @@
       <c r="AR112" s="1"/>
       <c r="AS112" s="1"/>
     </row>
-    <row r="113" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="65" t="s">
         <v>344</v>
       </c>
@@ -15670,7 +15672,7 @@
       <c r="AR113" s="1"/>
       <c r="AS113" s="1"/>
     </row>
-    <row r="114" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="65" t="s">
         <v>344</v>
       </c>
@@ -15737,7 +15739,7 @@
       <c r="AR114" s="1"/>
       <c r="AS114" s="1"/>
     </row>
-    <row r="115" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="65" t="s">
         <v>344</v>
       </c>
@@ -15805,7 +15807,7 @@
       <c r="AR115" s="1"/>
       <c r="AS115" s="1"/>
     </row>
-    <row r="116" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="65" t="s">
         <v>344</v>
       </c>
@@ -15872,7 +15874,7 @@
       <c r="AR116" s="1"/>
       <c r="AS116" s="1"/>
     </row>
-    <row r="117" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="65" t="s">
         <v>344</v>
       </c>
@@ -15940,7 +15942,7 @@
       <c r="AR117" s="1"/>
       <c r="AS117" s="1"/>
     </row>
-    <row r="118" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="65" t="s">
         <v>344</v>
       </c>
@@ -16007,7 +16009,7 @@
       <c r="AR118" s="1"/>
       <c r="AS118" s="1"/>
     </row>
-    <row r="119" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="65" t="s">
         <v>344</v>
       </c>
@@ -16074,7 +16076,7 @@
       <c r="AR119" s="1"/>
       <c r="AS119" s="1"/>
     </row>
-    <row r="120" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="65" t="s">
         <v>344</v>
       </c>
@@ -16141,7 +16143,7 @@
       <c r="AR120" s="1"/>
       <c r="AS120" s="1"/>
     </row>
-    <row r="121" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="65" t="s">
         <v>344</v>
       </c>
@@ -16208,7 +16210,7 @@
       <c r="AR121" s="1"/>
       <c r="AS121" s="1"/>
     </row>
-    <row r="122" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="65" t="s">
         <v>344</v>
       </c>
@@ -16275,7 +16277,7 @@
       <c r="AR122" s="1"/>
       <c r="AS122" s="1"/>
     </row>
-    <row r="123" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="65" t="s">
         <v>344</v>
       </c>
@@ -16342,7 +16344,7 @@
       <c r="AR123" s="1"/>
       <c r="AS123" s="1"/>
     </row>
-    <row r="124" spans="1:45" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:45" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="65" t="s">
         <v>344</v>
       </c>
@@ -16409,7 +16411,7 @@
       <c r="AR124" s="1"/>
       <c r="AS124" s="1"/>
     </row>
-    <row r="125" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="81" t="s">
         <v>193</v>
       </c>
@@ -16474,7 +16476,7 @@
       <c r="AR125" s="1"/>
       <c r="AS125" s="1"/>
     </row>
-    <row r="126" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="81" t="s">
         <v>345</v>
       </c>
@@ -16543,7 +16545,7 @@
       <c r="AR126" s="1"/>
       <c r="AS126" s="1"/>
     </row>
-    <row r="127" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="81" t="s">
         <v>345</v>
       </c>
@@ -16610,7 +16612,7 @@
       <c r="AR127" s="1"/>
       <c r="AS127" s="1"/>
     </row>
-    <row r="128" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="81" t="s">
         <v>345</v>
       </c>
@@ -16675,7 +16677,7 @@
       <c r="AR128" s="1"/>
       <c r="AS128" s="1"/>
     </row>
-    <row r="129" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="81" t="s">
         <v>345</v>
       </c>
@@ -16741,7 +16743,7 @@
       <c r="AR129" s="1"/>
       <c r="AS129" s="1"/>
     </row>
-    <row r="130" spans="1:45" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="81" t="s">
         <v>345</v>
       </c>
@@ -16821,7 +16823,7 @@
         <v>0</v>
       </c>
       <c r="E131" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F131" s="67" t="s">
         <v>218</v>
@@ -16891,7 +16893,7 @@
         <v>1</v>
       </c>
       <c r="E132" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F132" s="67" t="s">
         <v>219</v>
@@ -16961,7 +16963,7 @@
         <v>2</v>
       </c>
       <c r="E133" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F133" s="67" t="s">
         <v>220</v>
@@ -17031,7 +17033,7 @@
         <v>3</v>
       </c>
       <c r="E134" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F134" s="67" t="s">
         <v>221</v>
@@ -17101,7 +17103,7 @@
         <v>4</v>
       </c>
       <c r="E135" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F135" s="67" t="s">
         <v>222</v>
@@ -17171,7 +17173,7 @@
         <v>5</v>
       </c>
       <c r="E136" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F136" s="67" t="s">
         <v>223</v>
@@ -17241,7 +17243,7 @@
         <v>6</v>
       </c>
       <c r="E137" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F137" s="67" t="s">
         <v>224</v>
@@ -17311,7 +17313,7 @@
         <v>7</v>
       </c>
       <c r="E138" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F138" s="67" t="s">
         <v>227</v>
@@ -17381,7 +17383,7 @@
         <v>8</v>
       </c>
       <c r="E139" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F139" s="67" t="s">
         <v>338</v>
@@ -17451,7 +17453,7 @@
         <v>9</v>
       </c>
       <c r="E140" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F140" s="67" t="s">
         <v>339</v>
@@ -17521,7 +17523,7 @@
         <v>10</v>
       </c>
       <c r="E141" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F141" s="86" t="s">
         <v>346</v>
@@ -17563,7 +17565,7 @@
         <v>11</v>
       </c>
       <c r="E142" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F142" s="86" t="s">
         <v>348</v>
@@ -17605,7 +17607,7 @@
         <v>12</v>
       </c>
       <c r="E143" s="92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F143" s="86" t="s">
         <v>347</v>
@@ -17633,15 +17635,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N143" xr:uid="{58870481-4012-4967-9DF8-188DDC2BA7B8}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="1"/>
-        <filter val="2"/>
-        <filter val="3"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N143" xr:uid="{58870481-4012-4967-9DF8-188DDC2BA7B8}"/>
   <mergeCells count="4">
     <mergeCell ref="F95:F100"/>
     <mergeCell ref="F101:F103"/>
@@ -17675,8 +17669,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -17848,6 +17842,9 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -17856,8 +17853,17 @@
       <c r="B16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>251</v>
       </c>
@@ -17870,16 +17876,28 @@
       <c r="D17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>252</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>260</v>
       </c>
@@ -17887,7 +17905,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>261</v>
       </c>
@@ -17895,7 +17913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>262</v>
       </c>

</xml_diff>